<commit_message>
Created line plots for physiology and modified statistics output
</commit_message>
<xml_diff>
--- a/data/plant_physiology.xlsx
+++ b/data/plant_physiology.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacop\OneDrive\Desktop\Internship\sensors_analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F23CE75-01C6-4C6A-9D99-5885E4B62762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF8CD171-8747-454D-9301-1C6B36C70CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="21806" windowHeight="13886" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="21">
   <si>
     <t>date</t>
   </si>
@@ -71,6 +71,24 @@
   <si>
     <t>C3</t>
   </si>
+  <si>
+    <t>crown no.</t>
+  </si>
+  <si>
+    <t>vampiri no.</t>
+  </si>
+  <si>
+    <t>inflorescence no.</t>
+  </si>
+  <si>
+    <t>flower no.</t>
+  </si>
+  <si>
+    <t>fruit no.</t>
+  </si>
+  <si>
+    <t>4/23/2025</t>
+  </si>
 </sst>
 </file>
 
@@ -99,7 +117,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -221,11 +239,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -236,6 +306,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:K121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="N89" sqref="N89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -528,7 +603,7 @@
     <col min="6" max="6" width="20.921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,13 +617,28 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -562,13 +652,22 @@
         <v>1</v>
       </c>
       <c r="E2" s="5">
-        <v>11</v>
-      </c>
-      <c r="F2" s="6">
+        <v>3</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="6">
         <v>8.0555555559999998</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -582,13 +681,22 @@
         <v>2</v>
       </c>
       <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7">
+        <v>1</v>
+      </c>
+      <c r="G3" s="7">
         <v>5</v>
       </c>
-      <c r="F3" s="8">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="8">
         <v>9.26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
@@ -602,13 +710,22 @@
         <v>3</v>
       </c>
       <c r="E4" s="7">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7">
+        <v>6</v>
+      </c>
+      <c r="G4" s="7">
         <v>16</v>
       </c>
-      <c r="F4" s="8">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="8">
         <v>8.6214285709999992</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -622,13 +739,22 @@
         <v>4</v>
       </c>
       <c r="E5" s="7">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
         <v>9</v>
       </c>
-      <c r="F5" s="8">
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="8">
         <v>5.7888888889999999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" s="4" t="s">
         <v>6</v>
       </c>
@@ -642,13 +768,22 @@
         <v>5</v>
       </c>
       <c r="E6" s="7">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
         <v>10</v>
       </c>
-      <c r="F6" s="8">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="8">
         <v>6.91</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -661,14 +796,23 @@
       <c r="D7" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="5">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
         <v>8</v>
       </c>
-      <c r="F7" s="8">
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="8">
         <v>7.744444444</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -682,13 +826,22 @@
         <v>2</v>
       </c>
       <c r="E8" s="7">
+        <v>2</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
         <v>5</v>
       </c>
-      <c r="F8" s="8">
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="8">
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -702,13 +855,22 @@
         <v>3</v>
       </c>
       <c r="E9" s="7">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7">
+        <v>2</v>
+      </c>
+      <c r="G9" s="7">
         <v>14</v>
       </c>
-      <c r="F9" s="8">
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="8">
         <v>8.2583333329999995</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
@@ -722,13 +884,22 @@
         <v>4</v>
       </c>
       <c r="E10" s="7">
+        <v>3</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2</v>
+      </c>
+      <c r="G10" s="7">
         <v>12</v>
       </c>
-      <c r="F10" s="8">
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="8">
         <v>8.8000000000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" s="4" t="s">
         <v>6</v>
       </c>
@@ -742,13 +913,22 @@
         <v>5</v>
       </c>
       <c r="E11" s="7">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
         <v>9</v>
       </c>
-      <c r="F11" s="8">
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="8">
         <v>6.625</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" s="4" t="s">
         <v>6</v>
       </c>
@@ -761,14 +941,23 @@
       <c r="D12" s="5">
         <v>1</v>
       </c>
-      <c r="E12" s="7">
+      <c r="E12" s="5">
+        <v>2</v>
+      </c>
+      <c r="F12" s="5">
+        <v>4</v>
+      </c>
+      <c r="G12" s="7">
         <v>15</v>
       </c>
-      <c r="F12" s="8">
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="8">
         <v>8.309090909</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
@@ -782,13 +971,22 @@
         <v>2</v>
       </c>
       <c r="E13" s="7">
+        <v>2</v>
+      </c>
+      <c r="F13" s="7">
+        <v>0</v>
+      </c>
+      <c r="G13" s="7">
         <v>10</v>
       </c>
-      <c r="F13" s="8">
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="8">
         <v>8.65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
@@ -802,13 +1000,22 @@
         <v>3</v>
       </c>
       <c r="E14" s="7">
+        <v>3</v>
+      </c>
+      <c r="F14" s="7">
+        <v>4</v>
+      </c>
+      <c r="G14" s="7">
         <v>16</v>
       </c>
-      <c r="F14" s="8">
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="8">
         <v>9.9600000000000009</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
@@ -822,13 +1029,22 @@
         <v>4</v>
       </c>
       <c r="E15" s="7">
-        <v>11</v>
-      </c>
-      <c r="F15" s="8">
+        <v>3</v>
+      </c>
+      <c r="F15" s="7">
+        <v>1</v>
+      </c>
+      <c r="G15" s="7">
+        <v>11</v>
+      </c>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="8">
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
@@ -842,13 +1058,22 @@
         <v>5</v>
       </c>
       <c r="E16" s="7">
+        <v>3</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7">
         <v>12</v>
       </c>
-      <c r="F16" s="8">
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="8">
         <v>7.4545454549999999</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" s="4" t="s">
         <v>6</v>
       </c>
@@ -861,14 +1086,23 @@
       <c r="D17" s="5">
         <v>1</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="5">
+        <v>3</v>
+      </c>
+      <c r="F17" s="5">
+        <v>4</v>
+      </c>
+      <c r="G17" s="7">
         <v>18</v>
       </c>
-      <c r="F17" s="8">
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="8">
         <v>10.65714286</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" s="4" t="s">
         <v>6</v>
       </c>
@@ -882,13 +1116,22 @@
         <v>2</v>
       </c>
       <c r="E18" s="7">
+        <v>4</v>
+      </c>
+      <c r="F18" s="7">
+        <v>2</v>
+      </c>
+      <c r="G18" s="7">
         <v>14</v>
       </c>
-      <c r="F18" s="8">
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="8">
         <v>9.7833333329999999</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" s="4" t="s">
         <v>6</v>
       </c>
@@ -902,13 +1145,22 @@
         <v>3</v>
       </c>
       <c r="E19" s="7">
+        <v>4</v>
+      </c>
+      <c r="F19" s="7">
+        <v>4</v>
+      </c>
+      <c r="G19" s="7">
         <v>20</v>
       </c>
-      <c r="F19" s="8">
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="8">
         <v>7.7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -922,13 +1174,22 @@
         <v>4</v>
       </c>
       <c r="E20" s="7">
+        <v>3</v>
+      </c>
+      <c r="F20" s="7">
+        <v>2</v>
+      </c>
+      <c r="G20" s="7">
         <v>12</v>
       </c>
-      <c r="F20" s="8">
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="8">
         <v>9.2249999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
@@ -942,13 +1203,22 @@
         <v>5</v>
       </c>
       <c r="E21" s="7">
-        <v>11</v>
-      </c>
-      <c r="F21" s="8">
+        <v>3</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="7">
+        <v>11</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="8">
         <v>9.5545454549999995</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
         <v>6</v>
       </c>
@@ -961,14 +1231,23 @@
       <c r="D22" s="5">
         <v>1</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="5">
+        <v>3</v>
+      </c>
+      <c r="F22" s="5">
+        <v>3</v>
+      </c>
+      <c r="G22" s="7">
         <v>15</v>
       </c>
-      <c r="F22" s="8">
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="8">
         <v>9.2083333330000006</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A23" s="4" t="s">
         <v>6</v>
       </c>
@@ -982,13 +1261,22 @@
         <v>2</v>
       </c>
       <c r="E23" s="7">
+        <v>3</v>
+      </c>
+      <c r="F23" s="7">
+        <v>2</v>
+      </c>
+      <c r="G23" s="7">
         <v>10</v>
       </c>
-      <c r="F23" s="8">
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="8">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
@@ -1002,13 +1290,22 @@
         <v>3</v>
       </c>
       <c r="E24" s="7">
+        <v>4</v>
+      </c>
+      <c r="F24" s="7">
+        <v>0</v>
+      </c>
+      <c r="G24" s="7">
         <v>13</v>
       </c>
-      <c r="F24" s="8">
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="8">
         <v>10.425000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A25" s="4" t="s">
         <v>6</v>
       </c>
@@ -1022,13 +1319,22 @@
         <v>4</v>
       </c>
       <c r="E25" s="7">
+        <v>7</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0</v>
+      </c>
+      <c r="G25" s="7">
         <v>20</v>
       </c>
-      <c r="F25" s="8">
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="8">
         <v>8.7333333329999991</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
@@ -1042,13 +1348,22 @@
         <v>5</v>
       </c>
       <c r="E26" s="7">
-        <v>11</v>
-      </c>
-      <c r="F26" s="8">
+        <v>4</v>
+      </c>
+      <c r="F26" s="7">
+        <v>1</v>
+      </c>
+      <c r="G26" s="7">
+        <v>11</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="8">
         <v>8.0399999999999991</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A27" s="4" t="s">
         <v>6</v>
       </c>
@@ -1062,13 +1377,22 @@
         <v>1</v>
       </c>
       <c r="E27" s="7">
-        <v>11</v>
-      </c>
-      <c r="F27" s="8">
+        <v>3</v>
+      </c>
+      <c r="F27" s="7">
+        <v>0</v>
+      </c>
+      <c r="G27" s="7">
+        <v>11</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="8">
         <v>10.25</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A28" s="4" t="s">
         <v>6</v>
       </c>
@@ -1082,13 +1406,22 @@
         <v>2</v>
       </c>
       <c r="E28" s="7">
+        <v>4</v>
+      </c>
+      <c r="F28" s="7">
+        <v>3</v>
+      </c>
+      <c r="G28" s="7">
         <v>16</v>
       </c>
-      <c r="F28" s="8">
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="8">
         <v>11.476923080000001</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A29" s="4" t="s">
         <v>6</v>
       </c>
@@ -1102,13 +1435,22 @@
         <v>3</v>
       </c>
       <c r="E29" s="7">
+        <v>6</v>
+      </c>
+      <c r="F29" s="7">
+        <v>0</v>
+      </c>
+      <c r="G29" s="7">
         <v>13</v>
       </c>
-      <c r="F29" s="8">
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="8">
         <v>10.393333330000001</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A30" s="4" t="s">
         <v>6</v>
       </c>
@@ -1122,13 +1464,22 @@
         <v>4</v>
       </c>
       <c r="E30" s="7">
+        <v>3</v>
+      </c>
+      <c r="F30" s="7">
+        <v>1</v>
+      </c>
+      <c r="G30" s="7">
         <v>13</v>
       </c>
-      <c r="F30" s="8">
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="8">
         <v>9.0846153849999993</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A31" s="4" t="s">
         <v>6</v>
       </c>
@@ -1142,13 +1493,22 @@
         <v>5</v>
       </c>
       <c r="E31" s="7">
+        <v>3</v>
+      </c>
+      <c r="F31" s="7">
+        <v>0</v>
+      </c>
+      <c r="G31" s="7">
         <v>9</v>
       </c>
-      <c r="F31" s="8">
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="8">
         <v>8.511111111</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A32" s="9">
         <v>45934</v>
       </c>
@@ -1161,14 +1521,19 @@
       <c r="D32" s="5">
         <v>1</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7">
         <v>14</v>
       </c>
-      <c r="F32" s="8">
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="8">
         <v>12.32857143</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A33" s="9">
         <v>45934</v>
       </c>
@@ -1181,14 +1546,19 @@
       <c r="D33" s="7">
         <v>2</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7">
         <v>8</v>
       </c>
-      <c r="F33" s="8">
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="8">
         <v>16.190909090000002</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A34" s="9">
         <v>45934</v>
       </c>
@@ -1201,14 +1571,19 @@
       <c r="D34" s="7">
         <v>3</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7">
         <v>29</v>
       </c>
-      <c r="F34" s="8">
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="8">
         <v>15.804761900000001</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" s="9">
         <v>45934</v>
       </c>
@@ -1221,14 +1596,19 @@
       <c r="D35" s="7">
         <v>4</v>
       </c>
-      <c r="E35" s="7">
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7">
         <v>12</v>
       </c>
-      <c r="F35" s="8">
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="8">
         <v>14.75</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A36" s="9">
         <v>45934</v>
       </c>
@@ -1241,14 +1621,19 @@
       <c r="D36" s="7">
         <v>5</v>
       </c>
-      <c r="E36" s="7">
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7">
         <v>10</v>
       </c>
-      <c r="F36" s="8">
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="8">
         <v>13.955555560000001</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A37" s="9">
         <v>45934</v>
       </c>
@@ -1261,14 +1646,19 @@
       <c r="D37" s="5">
         <v>1</v>
       </c>
-      <c r="E37" s="7">
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7">
         <v>12</v>
       </c>
-      <c r="F37" s="8">
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="8">
         <v>15.175000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" s="9">
         <v>45934</v>
       </c>
@@ -1281,14 +1671,19 @@
       <c r="D38" s="7">
         <v>2</v>
       </c>
-      <c r="E38" s="7">
-        <v>7</v>
-      </c>
-      <c r="F38" s="8">
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7">
+        <v>7</v>
+      </c>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="8">
         <v>14.987500000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A39" s="9">
         <v>45934</v>
       </c>
@@ -1301,14 +1696,19 @@
       <c r="D39" s="7">
         <v>3</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7">
         <v>21</v>
       </c>
-      <c r="F39" s="8">
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="8">
         <v>13.17333333</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A40" s="9">
         <v>45934</v>
       </c>
@@ -1321,14 +1721,19 @@
       <c r="D40" s="7">
         <v>4</v>
       </c>
-      <c r="E40" s="7">
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7">
         <v>16</v>
       </c>
-      <c r="F40" s="8">
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="12"/>
+      <c r="K40" s="8">
         <v>14.758823530000001</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A41" s="9">
         <v>45934</v>
       </c>
@@ -1341,14 +1746,19 @@
       <c r="D41" s="7">
         <v>5</v>
       </c>
-      <c r="E41" s="7">
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7">
         <v>12</v>
       </c>
-      <c r="F41" s="8">
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="8">
         <v>12.08888889</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A42" s="9">
         <v>45934</v>
       </c>
@@ -1361,14 +1771,19 @@
       <c r="D42" s="5">
         <v>1</v>
       </c>
-      <c r="E42" s="7">
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7">
         <v>16</v>
       </c>
-      <c r="F42" s="8">
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="8">
         <v>14.483333330000001</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A43" s="9">
         <v>45934</v>
       </c>
@@ -1381,14 +1796,19 @@
       <c r="D43" s="7">
         <v>2</v>
       </c>
-      <c r="E43" s="7">
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7">
         <v>14</v>
       </c>
-      <c r="F43" s="8">
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="12"/>
+      <c r="K43" s="8">
         <v>13.74</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A44" s="9">
         <v>45934</v>
       </c>
@@ -1401,14 +1821,19 @@
       <c r="D44" s="7">
         <v>3</v>
       </c>
-      <c r="E44" s="7">
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7">
         <v>22</v>
       </c>
-      <c r="F44" s="8">
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="12"/>
+      <c r="K44" s="8">
         <v>15.114285710000001</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A45" s="9">
         <v>45934</v>
       </c>
@@ -1421,14 +1846,19 @@
       <c r="D45" s="7">
         <v>4</v>
       </c>
-      <c r="E45" s="7">
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7">
         <v>17</v>
       </c>
-      <c r="F45" s="8">
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="8">
         <v>15.32857143</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46" s="9">
         <v>45934</v>
       </c>
@@ -1441,14 +1871,19 @@
       <c r="D46" s="7">
         <v>5</v>
       </c>
-      <c r="E46" s="7">
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7">
         <v>16</v>
       </c>
-      <c r="F46" s="8">
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="8">
         <v>12.9</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A47" s="9">
         <v>45934</v>
       </c>
@@ -1461,14 +1896,19 @@
       <c r="D47" s="5">
         <v>1</v>
       </c>
-      <c r="E47" s="7">
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7">
         <v>24</v>
       </c>
-      <c r="F47" s="8">
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="8">
         <v>16.036363640000001</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A48" s="9">
         <v>45934</v>
       </c>
@@ -1481,14 +1921,19 @@
       <c r="D48" s="7">
         <v>2</v>
       </c>
-      <c r="E48" s="7">
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7">
         <v>22</v>
       </c>
-      <c r="F48" s="8">
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="12"/>
+      <c r="K48" s="8">
         <v>14.936842110000001</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A49" s="9">
         <v>45934</v>
       </c>
@@ -1501,14 +1946,19 @@
       <c r="D49" s="7">
         <v>3</v>
       </c>
-      <c r="E49" s="7">
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7">
         <v>23</v>
       </c>
-      <c r="F49" s="8">
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="12"/>
+      <c r="K49" s="8">
         <v>13.75714286</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A50" s="9">
         <v>45934</v>
       </c>
@@ -1521,14 +1971,19 @@
       <c r="D50" s="7">
         <v>4</v>
       </c>
-      <c r="E50" s="7">
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7">
         <v>18</v>
       </c>
-      <c r="F50" s="8">
+      <c r="H50" s="7"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="8">
         <v>16.3</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A51" s="9">
         <v>45934</v>
       </c>
@@ -1541,14 +1996,19 @@
       <c r="D51" s="7">
         <v>5</v>
       </c>
-      <c r="E51" s="7">
+      <c r="E51" s="7"/>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7">
         <v>16</v>
       </c>
-      <c r="F51" s="8">
+      <c r="H51" s="7"/>
+      <c r="I51" s="7"/>
+      <c r="J51" s="12"/>
+      <c r="K51" s="8">
         <v>16.514285709999999</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A52" s="9">
         <v>45934</v>
       </c>
@@ -1561,14 +2021,19 @@
       <c r="D52" s="5">
         <v>1</v>
       </c>
-      <c r="E52" s="7">
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7">
         <v>22</v>
       </c>
-      <c r="F52" s="8">
+      <c r="H52" s="7"/>
+      <c r="I52" s="7"/>
+      <c r="J52" s="12"/>
+      <c r="K52" s="8">
         <v>15.12</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A53" s="9">
         <v>45934</v>
       </c>
@@ -1581,14 +2046,19 @@
       <c r="D53" s="7">
         <v>2</v>
       </c>
-      <c r="E53" s="7">
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7">
         <v>19</v>
       </c>
-      <c r="F53" s="8">
+      <c r="H53" s="7"/>
+      <c r="I53" s="7"/>
+      <c r="J53" s="12"/>
+      <c r="K53" s="8">
         <v>17.443750000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A54" s="9">
         <v>45934</v>
       </c>
@@ -1601,14 +2071,19 @@
       <c r="D54" s="7">
         <v>3</v>
       </c>
-      <c r="E54" s="7">
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7">
         <v>21</v>
       </c>
-      <c r="F54" s="8">
+      <c r="H54" s="7"/>
+      <c r="I54" s="7"/>
+      <c r="J54" s="12"/>
+      <c r="K54" s="8">
         <v>16.043749999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A55" s="9">
         <v>45934</v>
       </c>
@@ -1621,14 +2096,19 @@
       <c r="D55" s="7">
         <v>4</v>
       </c>
-      <c r="E55" s="7">
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7">
         <v>28</v>
       </c>
-      <c r="F55" s="8">
+      <c r="H55" s="7"/>
+      <c r="I55" s="7"/>
+      <c r="J55" s="12"/>
+      <c r="K55" s="8">
         <v>13.922727269999999</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A56" s="9">
         <v>45934</v>
       </c>
@@ -1641,14 +2121,19 @@
       <c r="D56" s="7">
         <v>5</v>
       </c>
-      <c r="E56" s="7">
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7">
         <v>18</v>
       </c>
-      <c r="F56" s="8">
+      <c r="H56" s="7"/>
+      <c r="I56" s="7"/>
+      <c r="J56" s="12"/>
+      <c r="K56" s="8">
         <v>13.53333333</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A57" s="9">
         <v>45934</v>
       </c>
@@ -1661,14 +2146,19 @@
       <c r="D57" s="7">
         <v>1</v>
       </c>
-      <c r="E57" s="7">
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7">
         <v>16</v>
       </c>
-      <c r="F57" s="8">
+      <c r="H57" s="7"/>
+      <c r="I57" s="7"/>
+      <c r="J57" s="12"/>
+      <c r="K57" s="8">
         <v>13.97142857</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A58" s="9">
         <v>45934</v>
       </c>
@@ -1681,14 +2171,19 @@
       <c r="D58" s="7">
         <v>2</v>
       </c>
-      <c r="E58" s="7">
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7">
         <v>20</v>
       </c>
-      <c r="F58" s="8">
+      <c r="H58" s="7"/>
+      <c r="I58" s="7"/>
+      <c r="J58" s="12"/>
+      <c r="K58" s="8">
         <v>16.375</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A59" s="9">
         <v>45934</v>
       </c>
@@ -1701,14 +2196,19 @@
       <c r="D59" s="7">
         <v>3</v>
       </c>
-      <c r="E59" s="7">
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7">
         <v>22</v>
       </c>
-      <c r="F59" s="8">
+      <c r="H59" s="7"/>
+      <c r="I59" s="7"/>
+      <c r="J59" s="12"/>
+      <c r="K59" s="8">
         <v>15.705</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A60" s="9">
         <v>45934</v>
       </c>
@@ -1721,14 +2221,19 @@
       <c r="D60" s="7">
         <v>4</v>
       </c>
-      <c r="E60" s="7">
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7">
         <v>20</v>
       </c>
-      <c r="F60" s="8">
+      <c r="H60" s="7"/>
+      <c r="I60" s="7"/>
+      <c r="J60" s="12"/>
+      <c r="K60" s="8">
         <v>13.65625</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A61" s="9">
         <v>45934</v>
       </c>
@@ -1741,11 +2246,1816 @@
       <c r="D61" s="7">
         <v>5</v>
       </c>
-      <c r="E61" s="7">
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7">
         <v>12</v>
       </c>
-      <c r="F61" s="8">
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+      <c r="J61" s="12"/>
+      <c r="K61" s="8">
         <v>13.490909090000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A62" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D62" s="5">
+        <v>1</v>
+      </c>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7">
+        <v>21</v>
+      </c>
+      <c r="H62" s="7">
+        <v>3</v>
+      </c>
+      <c r="I62" s="7">
+        <v>5</v>
+      </c>
+      <c r="J62" s="12"/>
+      <c r="K62" s="8">
+        <v>21.470833330000001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A63" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D63" s="7">
+        <v>2</v>
+      </c>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7">
+        <v>14</v>
+      </c>
+      <c r="H63" s="7">
+        <v>2</v>
+      </c>
+      <c r="I63" s="7">
+        <v>3</v>
+      </c>
+      <c r="J63" s="12"/>
+      <c r="K63" s="8">
+        <v>23.172727269999999</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A64" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D64" s="7">
+        <v>3</v>
+      </c>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7">
+        <v>40</v>
+      </c>
+      <c r="H64" s="7">
+        <v>10</v>
+      </c>
+      <c r="I64" s="7">
+        <v>4</v>
+      </c>
+      <c r="J64" s="12"/>
+      <c r="K64" s="8">
+        <v>23.964285709999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A65" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" s="7">
+        <v>4</v>
+      </c>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7">
+        <v>23</v>
+      </c>
+      <c r="H65" s="7">
+        <v>4</v>
+      </c>
+      <c r="I65" s="7">
+        <v>5</v>
+      </c>
+      <c r="J65" s="12"/>
+      <c r="K65" s="8">
+        <v>24.85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A66" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" s="7">
+        <v>5</v>
+      </c>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7">
+        <v>19</v>
+      </c>
+      <c r="H66" s="7">
+        <v>3</v>
+      </c>
+      <c r="I66" s="7">
+        <v>6</v>
+      </c>
+      <c r="J66" s="12"/>
+      <c r="K66" s="8">
+        <v>23.58888889</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A67" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" s="5">
+        <v>1</v>
+      </c>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7">
+        <v>21</v>
+      </c>
+      <c r="H67" s="7">
+        <v>5</v>
+      </c>
+      <c r="I67" s="7">
+        <v>4</v>
+      </c>
+      <c r="J67" s="12"/>
+      <c r="K67" s="8">
+        <v>21.975000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A68" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" s="7">
+        <v>2</v>
+      </c>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7">
+        <v>14</v>
+      </c>
+      <c r="H68" s="7">
+        <v>2</v>
+      </c>
+      <c r="I68" s="7">
+        <v>6</v>
+      </c>
+      <c r="J68" s="12"/>
+      <c r="K68" s="8">
+        <v>25.64545455</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A69" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="7">
+        <v>3</v>
+      </c>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7">
+        <v>26</v>
+      </c>
+      <c r="H69" s="7">
+        <v>4</v>
+      </c>
+      <c r="I69" s="7">
+        <v>10</v>
+      </c>
+      <c r="J69" s="12"/>
+      <c r="K69" s="8">
+        <v>23.081250000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A70" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" s="7">
+        <v>4</v>
+      </c>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7">
+        <v>28</v>
+      </c>
+      <c r="H70" s="7">
+        <v>7</v>
+      </c>
+      <c r="I70" s="7">
+        <v>10</v>
+      </c>
+      <c r="J70" s="12"/>
+      <c r="K70" s="8">
+        <v>26.388235290000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A71" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" s="7">
+        <v>5</v>
+      </c>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7">
+        <v>17</v>
+      </c>
+      <c r="H71" s="7">
+        <v>2</v>
+      </c>
+      <c r="I71" s="7">
+        <v>6</v>
+      </c>
+      <c r="J71" s="12"/>
+      <c r="K71" s="8">
+        <v>25.61538462</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A72" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D72" s="5">
+        <v>1</v>
+      </c>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7">
+        <v>24</v>
+      </c>
+      <c r="H72" s="7">
+        <v>9</v>
+      </c>
+      <c r="I72" s="7">
+        <v>8</v>
+      </c>
+      <c r="J72" s="12"/>
+      <c r="K72" s="8">
+        <v>26.15909091</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A73" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D73" s="7">
+        <v>2</v>
+      </c>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7">
+        <v>17</v>
+      </c>
+      <c r="H73" s="7">
+        <v>3</v>
+      </c>
+      <c r="I73" s="7">
+        <v>7</v>
+      </c>
+      <c r="J73" s="12"/>
+      <c r="K73" s="8">
+        <v>25.871428569999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A74" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D74" s="7">
+        <v>3</v>
+      </c>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7">
+        <v>28</v>
+      </c>
+      <c r="H74" s="7">
+        <v>5</v>
+      </c>
+      <c r="I74" s="7">
+        <v>9</v>
+      </c>
+      <c r="J74" s="12"/>
+      <c r="K74" s="8">
+        <v>25.15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A75" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D75" s="7">
+        <v>4</v>
+      </c>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7">
+        <v>22</v>
+      </c>
+      <c r="H75" s="7">
+        <v>4</v>
+      </c>
+      <c r="I75" s="7">
+        <v>14</v>
+      </c>
+      <c r="J75" s="12"/>
+      <c r="K75" s="8">
+        <v>24.561111109999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A76" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D76" s="7">
+        <v>5</v>
+      </c>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7">
+        <v>24</v>
+      </c>
+      <c r="H76" s="7">
+        <v>3</v>
+      </c>
+      <c r="I76" s="7">
+        <v>9</v>
+      </c>
+      <c r="J76" s="12"/>
+      <c r="K76" s="8">
+        <v>24.641176470000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A77" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" s="5">
+        <v>1</v>
+      </c>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7">
+        <v>29</v>
+      </c>
+      <c r="H77" s="7">
+        <v>8</v>
+      </c>
+      <c r="I77" s="7">
+        <v>7</v>
+      </c>
+      <c r="J77" s="12"/>
+      <c r="K77" s="8">
+        <v>24.62</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A78" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" s="7">
+        <v>2</v>
+      </c>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7">
+        <v>28</v>
+      </c>
+      <c r="H78" s="7">
+        <v>5</v>
+      </c>
+      <c r="I78" s="7">
+        <v>13</v>
+      </c>
+      <c r="J78" s="12"/>
+      <c r="K78" s="8">
+        <v>25.962068970000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A79" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" s="7">
+        <v>3</v>
+      </c>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7">
+        <v>32</v>
+      </c>
+      <c r="H79" s="7">
+        <v>8</v>
+      </c>
+      <c r="I79" s="7">
+        <v>11</v>
+      </c>
+      <c r="J79" s="12"/>
+      <c r="K79" s="8">
+        <v>25.54137931</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A80" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D80" s="7">
+        <v>4</v>
+      </c>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7">
+        <v>22</v>
+      </c>
+      <c r="H80" s="7">
+        <v>5</v>
+      </c>
+      <c r="I80" s="7">
+        <v>4</v>
+      </c>
+      <c r="J80" s="12"/>
+      <c r="K80" s="8">
+        <v>24.06</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A81" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D81" s="7">
+        <v>5</v>
+      </c>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7">
+        <v>23</v>
+      </c>
+      <c r="H81" s="7">
+        <v>3</v>
+      </c>
+      <c r="I81" s="7">
+        <v>6</v>
+      </c>
+      <c r="J81" s="12"/>
+      <c r="K81" s="8">
+        <v>25.81363636</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A82" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D82" s="5">
+        <v>1</v>
+      </c>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7">
+        <v>34</v>
+      </c>
+      <c r="H82" s="7">
+        <v>7</v>
+      </c>
+      <c r="I82" s="7">
+        <v>9</v>
+      </c>
+      <c r="J82" s="12"/>
+      <c r="K82" s="8">
+        <v>25.078260870000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A83" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D83" s="7">
+        <v>2</v>
+      </c>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7">
+        <v>26</v>
+      </c>
+      <c r="H83" s="7">
+        <v>5</v>
+      </c>
+      <c r="I83" s="7">
+        <v>9</v>
+      </c>
+      <c r="J83" s="12"/>
+      <c r="K83" s="8">
+        <v>24.40555556</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A84" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D84" s="7">
+        <v>3</v>
+      </c>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7">
+        <v>25</v>
+      </c>
+      <c r="H84" s="7">
+        <v>5</v>
+      </c>
+      <c r="I84" s="7">
+        <v>6</v>
+      </c>
+      <c r="J84" s="12"/>
+      <c r="K84" s="8">
+        <v>26.3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A85" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D85" s="7">
+        <v>4</v>
+      </c>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7">
+        <v>32</v>
+      </c>
+      <c r="H85" s="7">
+        <v>7</v>
+      </c>
+      <c r="I85" s="7">
+        <v>19</v>
+      </c>
+      <c r="J85" s="12"/>
+      <c r="K85" s="8">
+        <v>27.623809519999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A86" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D86" s="7">
+        <v>5</v>
+      </c>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7">
+        <v>27</v>
+      </c>
+      <c r="H86" s="7">
+        <v>6</v>
+      </c>
+      <c r="I86" s="7">
+        <v>8</v>
+      </c>
+      <c r="J86" s="12"/>
+      <c r="K86" s="8">
+        <v>23.8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A87" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B87" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D87" s="7">
+        <v>1</v>
+      </c>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7">
+        <v>22</v>
+      </c>
+      <c r="H87" s="7">
+        <v>5</v>
+      </c>
+      <c r="I87" s="7">
+        <v>8</v>
+      </c>
+      <c r="J87" s="12"/>
+      <c r="K87" s="8">
+        <v>24.085714289999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A88" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="7">
+        <v>2</v>
+      </c>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7">
+        <v>21</v>
+      </c>
+      <c r="H88" s="7">
+        <v>7</v>
+      </c>
+      <c r="I88" s="7">
+        <v>13</v>
+      </c>
+      <c r="J88" s="12"/>
+      <c r="K88" s="8">
+        <v>24.155000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A89" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="7">
+        <v>3</v>
+      </c>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7">
+        <v>24</v>
+      </c>
+      <c r="H89" s="7">
+        <v>8</v>
+      </c>
+      <c r="I89" s="7">
+        <v>9</v>
+      </c>
+      <c r="J89" s="12"/>
+      <c r="K89" s="8">
+        <v>25.32222222</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A90" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D90" s="7">
+        <v>4</v>
+      </c>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7">
+        <v>23</v>
+      </c>
+      <c r="H90" s="7">
+        <v>4</v>
+      </c>
+      <c r="I90" s="7">
+        <v>14</v>
+      </c>
+      <c r="J90" s="12"/>
+      <c r="K90" s="8">
+        <v>24.004545449999998</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A91" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="7">
+        <v>5</v>
+      </c>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7">
+        <v>21</v>
+      </c>
+      <c r="H91" s="7">
+        <v>3</v>
+      </c>
+      <c r="I91" s="7">
+        <v>7</v>
+      </c>
+      <c r="J91" s="12"/>
+      <c r="K91" s="8">
+        <v>23.329411759999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A92" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D92" s="5">
+        <v>1</v>
+      </c>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7">
+        <v>20</v>
+      </c>
+      <c r="H92" s="7">
+        <v>8</v>
+      </c>
+      <c r="I92" s="7">
+        <v>8</v>
+      </c>
+      <c r="J92" s="12">
+        <v>19</v>
+      </c>
+      <c r="K92" s="8">
+        <v>35.6</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A93" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D93" s="7">
+        <v>2</v>
+      </c>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7">
+        <v>16</v>
+      </c>
+      <c r="H93" s="7">
+        <v>3</v>
+      </c>
+      <c r="I93" s="7">
+        <v>1</v>
+      </c>
+      <c r="J93" s="12">
+        <v>13</v>
+      </c>
+      <c r="K93" s="8">
+        <v>31.18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A94" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" s="7">
+        <v>3</v>
+      </c>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7">
+        <v>56</v>
+      </c>
+      <c r="H94" s="7">
+        <v>12</v>
+      </c>
+      <c r="I94" s="7">
+        <v>20</v>
+      </c>
+      <c r="J94" s="12">
+        <v>36</v>
+      </c>
+      <c r="K94" s="8">
+        <v>34.76</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A95" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" s="7">
+        <v>4</v>
+      </c>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7">
+        <v>28</v>
+      </c>
+      <c r="H95" s="7">
+        <v>6</v>
+      </c>
+      <c r="I95" s="7">
+        <v>4</v>
+      </c>
+      <c r="J95" s="12">
+        <v>22</v>
+      </c>
+      <c r="K95" s="8">
+        <v>35.119999999999997</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A96" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D96" s="7">
+        <v>5</v>
+      </c>
+      <c r="E96" s="7"/>
+      <c r="F96" s="7"/>
+      <c r="G96" s="7">
+        <v>19</v>
+      </c>
+      <c r="H96" s="7">
+        <v>4</v>
+      </c>
+      <c r="I96" s="7">
+        <v>1</v>
+      </c>
+      <c r="J96" s="12">
+        <v>20</v>
+      </c>
+      <c r="K96" s="8">
+        <v>30.98</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A97" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97" s="5">
+        <v>1</v>
+      </c>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7">
+        <v>22</v>
+      </c>
+      <c r="H97" s="7">
+        <v>6</v>
+      </c>
+      <c r="I97" s="7">
+        <v>10</v>
+      </c>
+      <c r="J97" s="12">
+        <v>17</v>
+      </c>
+      <c r="K97" s="8">
+        <v>29.84</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A98" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" s="7">
+        <v>2</v>
+      </c>
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="7">
+        <v>15</v>
+      </c>
+      <c r="H98" s="7">
+        <v>3</v>
+      </c>
+      <c r="I98" s="7">
+        <v>2</v>
+      </c>
+      <c r="J98" s="12">
+        <v>12</v>
+      </c>
+      <c r="K98" s="8">
+        <v>37.159999999999997</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A99" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C99" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" s="7">
+        <v>3</v>
+      </c>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="7">
+        <v>24</v>
+      </c>
+      <c r="H99" s="7">
+        <v>10</v>
+      </c>
+      <c r="I99" s="7">
+        <v>6</v>
+      </c>
+      <c r="J99" s="12">
+        <v>21</v>
+      </c>
+      <c r="K99" s="8">
+        <v>26.72</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A100" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100" s="7">
+        <v>4</v>
+      </c>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7">
+        <v>36</v>
+      </c>
+      <c r="H100" s="7">
+        <v>8</v>
+      </c>
+      <c r="I100" s="7">
+        <v>12</v>
+      </c>
+      <c r="J100" s="12">
+        <v>34</v>
+      </c>
+      <c r="K100" s="8">
+        <v>33.9</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A101" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" s="7">
+        <v>5</v>
+      </c>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7">
+        <v>20</v>
+      </c>
+      <c r="H101" s="7">
+        <v>7</v>
+      </c>
+      <c r="I101" s="7">
+        <v>7</v>
+      </c>
+      <c r="J101" s="12">
+        <v>15</v>
+      </c>
+      <c r="K101" s="8">
+        <v>32.58</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A102" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B102" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D102" s="5">
+        <v>1</v>
+      </c>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7">
+        <v>30</v>
+      </c>
+      <c r="H102" s="7">
+        <v>8</v>
+      </c>
+      <c r="I102" s="7">
+        <v>13</v>
+      </c>
+      <c r="J102" s="12">
+        <v>18</v>
+      </c>
+      <c r="K102" s="8">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A103" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D103" s="7">
+        <v>2</v>
+      </c>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7">
+        <v>20</v>
+      </c>
+      <c r="H103" s="7">
+        <v>7</v>
+      </c>
+      <c r="I103" s="7">
+        <v>8</v>
+      </c>
+      <c r="J103" s="12">
+        <v>19</v>
+      </c>
+      <c r="K103" s="8">
+        <v>34.24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A104" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D104" s="7">
+        <v>3</v>
+      </c>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
+      <c r="G104" s="7">
+        <v>37</v>
+      </c>
+      <c r="H104" s="7">
+        <v>13</v>
+      </c>
+      <c r="I104" s="7">
+        <v>11</v>
+      </c>
+      <c r="J104" s="12">
+        <v>36</v>
+      </c>
+      <c r="K104" s="8">
+        <v>34.56</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A105" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D105" s="7">
+        <v>4</v>
+      </c>
+      <c r="E105" s="7"/>
+      <c r="F105" s="7"/>
+      <c r="G105" s="7">
+        <v>19</v>
+      </c>
+      <c r="H105" s="7">
+        <v>9</v>
+      </c>
+      <c r="I105" s="7">
+        <v>8</v>
+      </c>
+      <c r="J105" s="12">
+        <v>24</v>
+      </c>
+      <c r="K105" s="8">
+        <v>31.62</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A106" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D106" s="7">
+        <v>5</v>
+      </c>
+      <c r="E106" s="7"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="7">
+        <v>29</v>
+      </c>
+      <c r="H106" s="7">
+        <v>9</v>
+      </c>
+      <c r="I106" s="7">
+        <v>8</v>
+      </c>
+      <c r="J106" s="12">
+        <v>26</v>
+      </c>
+      <c r="K106" s="8">
+        <v>34.94</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A107" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D107" s="5">
+        <v>1</v>
+      </c>
+      <c r="E107" s="7"/>
+      <c r="F107" s="7"/>
+      <c r="G107" s="7">
+        <v>40</v>
+      </c>
+      <c r="H107" s="7">
+        <v>9</v>
+      </c>
+      <c r="I107" s="7">
+        <v>11</v>
+      </c>
+      <c r="J107" s="12">
+        <v>34</v>
+      </c>
+      <c r="K107" s="8">
+        <v>32.44</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A108" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D108" s="7">
+        <v>2</v>
+      </c>
+      <c r="E108" s="7"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="7">
+        <v>36</v>
+      </c>
+      <c r="H108" s="7">
+        <v>10</v>
+      </c>
+      <c r="I108" s="7">
+        <v>11</v>
+      </c>
+      <c r="J108" s="12">
+        <v>36</v>
+      </c>
+      <c r="K108" s="8">
+        <v>32.119999999999997</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A109" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D109" s="7">
+        <v>3</v>
+      </c>
+      <c r="E109" s="7"/>
+      <c r="F109" s="7"/>
+      <c r="G109" s="7">
+        <v>39</v>
+      </c>
+      <c r="H109" s="7">
+        <v>9</v>
+      </c>
+      <c r="I109" s="7">
+        <v>9</v>
+      </c>
+      <c r="J109" s="12">
+        <v>34</v>
+      </c>
+      <c r="K109" s="8">
+        <v>32.22</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A110" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D110" s="7">
+        <v>4</v>
+      </c>
+      <c r="E110" s="7"/>
+      <c r="F110" s="7"/>
+      <c r="G110" s="7">
+        <v>30</v>
+      </c>
+      <c r="H110" s="7">
+        <v>5</v>
+      </c>
+      <c r="I110" s="7">
+        <v>2</v>
+      </c>
+      <c r="J110" s="12">
+        <v>30</v>
+      </c>
+      <c r="K110" s="8">
+        <v>35.159999999999997</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A111" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D111" s="7">
+        <v>5</v>
+      </c>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7"/>
+      <c r="G111" s="7">
+        <v>23</v>
+      </c>
+      <c r="H111" s="7">
+        <v>6</v>
+      </c>
+      <c r="I111" s="7">
+        <v>8</v>
+      </c>
+      <c r="J111" s="12">
+        <v>23</v>
+      </c>
+      <c r="K111" s="8">
+        <v>33.880000000000003</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A112" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D112" s="5">
+        <v>1</v>
+      </c>
+      <c r="E112" s="7"/>
+      <c r="F112" s="7"/>
+      <c r="G112" s="7">
+        <v>35</v>
+      </c>
+      <c r="H112" s="7">
+        <v>12</v>
+      </c>
+      <c r="I112" s="7">
+        <v>16</v>
+      </c>
+      <c r="J112" s="12">
+        <v>37</v>
+      </c>
+      <c r="K112" s="8">
+        <v>36.979999999999997</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A113" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D113" s="7">
+        <v>2</v>
+      </c>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
+      <c r="G113" s="7">
+        <v>31</v>
+      </c>
+      <c r="H113" s="7">
+        <v>3</v>
+      </c>
+      <c r="I113" s="7">
+        <v>2</v>
+      </c>
+      <c r="J113" s="12">
+        <v>11</v>
+      </c>
+      <c r="K113" s="8">
+        <v>29.98</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A114" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D114" s="7">
+        <v>3</v>
+      </c>
+      <c r="E114" s="7"/>
+      <c r="F114" s="7"/>
+      <c r="G114" s="7">
+        <v>43</v>
+      </c>
+      <c r="H114" s="7">
+        <v>8</v>
+      </c>
+      <c r="I114" s="7">
+        <v>5</v>
+      </c>
+      <c r="J114" s="12">
+        <v>33</v>
+      </c>
+      <c r="K114" s="8">
+        <v>33.020000000000003</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A115" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D115" s="7">
+        <v>4</v>
+      </c>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7"/>
+      <c r="G115" s="7">
+        <v>27</v>
+      </c>
+      <c r="H115" s="7">
+        <v>9</v>
+      </c>
+      <c r="I115" s="7">
+        <v>3</v>
+      </c>
+      <c r="J115" s="12">
+        <v>46</v>
+      </c>
+      <c r="K115" s="8">
+        <v>37.54</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A116" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D116" s="7">
+        <v>5</v>
+      </c>
+      <c r="E116" s="7"/>
+      <c r="F116" s="7"/>
+      <c r="G116" s="7">
+        <v>31</v>
+      </c>
+      <c r="H116" s="7">
+        <v>11</v>
+      </c>
+      <c r="I116" s="7">
+        <v>9</v>
+      </c>
+      <c r="J116" s="12">
+        <v>33</v>
+      </c>
+      <c r="K116" s="8">
+        <v>32.72</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A117" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D117" s="7">
+        <v>1</v>
+      </c>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7"/>
+      <c r="G117" s="7">
+        <v>19</v>
+      </c>
+      <c r="H117" s="7">
+        <v>4</v>
+      </c>
+      <c r="I117" s="7">
+        <v>1</v>
+      </c>
+      <c r="J117" s="12">
+        <v>28</v>
+      </c>
+      <c r="K117" s="8">
+        <v>34.74</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A118" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D118" s="7">
+        <v>2</v>
+      </c>
+      <c r="E118" s="7"/>
+      <c r="F118" s="7"/>
+      <c r="G118" s="7">
+        <v>33</v>
+      </c>
+      <c r="H118" s="7">
+        <v>6</v>
+      </c>
+      <c r="I118" s="7">
+        <v>4</v>
+      </c>
+      <c r="J118" s="12">
+        <v>31</v>
+      </c>
+      <c r="K118" s="8">
+        <v>35.299999999999997</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A119" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D119" s="7">
+        <v>3</v>
+      </c>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7"/>
+      <c r="G119" s="7">
+        <v>26</v>
+      </c>
+      <c r="H119" s="7">
+        <v>12</v>
+      </c>
+      <c r="I119" s="7">
+        <v>8</v>
+      </c>
+      <c r="J119" s="12">
+        <v>47</v>
+      </c>
+      <c r="K119" s="8">
+        <v>34.659999999999997</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A120" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D120" s="7">
+        <v>4</v>
+      </c>
+      <c r="E120" s="7"/>
+      <c r="F120" s="7"/>
+      <c r="G120" s="7">
+        <v>26</v>
+      </c>
+      <c r="H120" s="7">
+        <v>8</v>
+      </c>
+      <c r="I120" s="7">
+        <v>7</v>
+      </c>
+      <c r="J120" s="12">
+        <v>23</v>
+      </c>
+      <c r="K120" s="8">
+        <v>35.28</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A121" s="14">
+        <v>45874</v>
+      </c>
+      <c r="B121" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D121" s="7">
+        <v>5</v>
+      </c>
+      <c r="E121" s="7"/>
+      <c r="F121" s="7"/>
+      <c r="G121" s="7">
+        <v>17</v>
+      </c>
+      <c r="H121" s="7">
+        <v>9</v>
+      </c>
+      <c r="I121" s="7">
+        <v>7</v>
+      </c>
+      <c r="J121" s="12">
+        <v>23</v>
+      </c>
+      <c r="K121" s="8">
+        <v>31.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>